<commit_message>
The model works, and there is a connection between all the three views (hubs, demand and company
Based on a goal share of demand that goes through the hub, the system achieves a state where the number of hubs is optimal using the funds based on the gap between the true share of demand and the goal. The innovation diffusion theory is applied to the company side only.
</commit_message>
<xml_diff>
--- a/Exogenous values.xlsx
+++ b/Exogenous values.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10901"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiaandruetto/Documents/HubsModel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ug.kth.se\dfs\home\a\n\andru\appdata\xp.V2\Documents\GitHub\HubsModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4C558F-9463-164C-A5D0-89FDA310407D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31520" yWindow="-660" windowWidth="28040" windowHeight="16940" activeTab="1" xr2:uid="{7E14CD48-C6EF-524C-97AC-20EBF6EEA564}"/>
+    <workbookView xWindow="-31515" yWindow="-660" windowWidth="28035" windowHeight="16935" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="company" sheetId="1" r:id="rId1"/>
     <sheet name="hubs" sheetId="2" r:id="rId2"/>
+    <sheet name="demand" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>total number of companies</t>
   </si>
@@ -51,12 +51,30 @@
   </si>
   <si>
     <t>maximum funds per unit of time</t>
+  </si>
+  <si>
+    <t>total demand</t>
+  </si>
+  <si>
+    <t>single hub capacity</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>Box/Hub</t>
+  </si>
+  <si>
+    <t>goal</t>
+  </si>
+  <si>
+    <t>Dmnl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -401,19 +419,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197579BB-F3D0-2545-B718-69CF9C3C23B5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,7 +439,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -429,7 +447,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -443,19 +461,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191107FC-2FBF-EF4B-8E68-E98BF3549123}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -463,12 +481,63 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
         <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>10000</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>0.6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented some cost structure
I have implemented a basic cost structure based on efficiency in routing and consolidation (positive effect) and based on cost of the hub (and how this is shared between the companies).
The part of the model that considers the positive effects does not work as wanted, still some time in the implementation of this is needed
</commit_message>
<xml_diff>
--- a/Exogenous values.xlsx
+++ b/Exogenous values.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31515" yWindow="-660" windowWidth="28035" windowHeight="16935" activeTab="2"/>
+    <workbookView xWindow="-31515" yWindow="-660" windowWidth="28035" windowHeight="16935" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="company" sheetId="1" r:id="rId1"/>
     <sheet name="hubs" sheetId="2" r:id="rId2"/>
     <sheet name="demand" sheetId="3" r:id="rId3"/>
+    <sheet name="cost" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>total number of companies</t>
   </si>
@@ -69,6 +70,24 @@
   </si>
   <si>
     <t>Dmnl</t>
+  </si>
+  <si>
+    <t>hubs location variable</t>
+  </si>
+  <si>
+    <t>initial routing and consolidation efficiency</t>
+  </si>
+  <si>
+    <t>total operation cost of one hub</t>
+  </si>
+  <si>
+    <t>[0,1]</t>
+  </si>
+  <si>
+    <t>$/Month</t>
+  </si>
+  <si>
+    <t>operation cost</t>
   </si>
 </sst>
 </file>
@@ -498,7 +517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -543,4 +562,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1">
+        <v>0.7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>0.6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed the way the efficiency works
Changed the effect of routing and consolidation efficiency so that it is actually a monetary value that depends on the efficiency itself (more mathematically correct) .
Also corrected the share of demand (before it was getting to more than 1!!!)
Corrected the number of hubs, so that it is always an integer
Added the monetary value as a value that influences the company adoption rate, in a way that it is still doubtful.....

Still TBD: add the CO2 emissions gap and try to understand how to make it so that the existing hubs need to be full before a new hub is purchased
</commit_message>
<xml_diff>
--- a/Exogenous values.xlsx
+++ b/Exogenous values.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31515" yWindow="-660" windowWidth="28035" windowHeight="16935" activeTab="3"/>
+    <workbookView xWindow="-31515" yWindow="-660" windowWidth="28035" windowHeight="9420" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="company" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>total number of companies</t>
   </si>
@@ -45,9 +45,6 @@
     <t>company contact rate</t>
   </si>
   <si>
-    <t>company adoption fraction</t>
-  </si>
-  <si>
     <t>building cost of hubs</t>
   </si>
   <si>
@@ -87,7 +84,13 @@
     <t>$/Month</t>
   </si>
   <si>
-    <t>operation cost</t>
+    <t>minimum operation cost</t>
+  </si>
+  <si>
+    <t>initial push time</t>
+  </si>
+  <si>
+    <t>initial company adoption fraction</t>
   </si>
 </sst>
 </file>
@@ -439,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -468,10 +471,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -494,7 +505,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1">
         <v>100000</v>
@@ -502,7 +513,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>10000</v>
@@ -518,7 +529,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -528,35 +539,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1">
         <v>10000</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>1000</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>0.6</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -569,7 +580,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -579,52 +590,52 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1">
         <v>0.7</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>0.6</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>1000</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added utilisation rate variable
Added a variable that accounts for how much the hub system is utilised, so that you don't get hubs when there are still many that are not used enough
</commit_message>
<xml_diff>
--- a/Exogenous values.xlsx
+++ b/Exogenous values.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31515" yWindow="-660" windowWidth="28035" windowHeight="9420" activeTab="3"/>
+    <workbookView xWindow="-31515" yWindow="-660" windowWidth="28035" windowHeight="9420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="company" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>total number of companies</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t>CO2/box</t>
+  </si>
+  <si>
+    <t>goal of co2 emissions</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>minimum utilization rate</t>
   </si>
 </sst>
 </file>
@@ -502,10 +511,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -513,7 +522,7 @@
     <col min="1" max="1" width="28.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -521,12 +530,23 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
         <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>0.6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -589,7 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -655,10 +675,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -688,6 +708,17 @@
         <v>20</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>1000000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed some units and added *SOME* descriptions for variables
Only added some of the descriptions. Still most of them NEED TO BE DONE!
</commit_message>
<xml_diff>
--- a/Exogenous values.xlsx
+++ b/Exogenous values.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31515" yWindow="-660" windowWidth="28035" windowHeight="9420" activeTab="1"/>
+    <workbookView xWindow="-31512" yWindow="-660" windowWidth="28032" windowHeight="9420" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="company" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>total number of companies</t>
   </si>
@@ -110,6 +110,21 @@
   </si>
   <si>
     <t>minimum utilization rate</t>
+  </si>
+  <si>
+    <t>companies</t>
+  </si>
+  <si>
+    <t>dmnl</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>$/hub</t>
+  </si>
+  <si>
+    <t>$/month</t>
   </si>
 </sst>
 </file>
@@ -461,47 +476,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4">
         <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -513,32 +540,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1">
         <v>100000</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
         <v>10000</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -559,15 +592,15 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -578,7 +611,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -589,7 +622,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -610,15 +643,15 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -632,7 +665,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -646,18 +679,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -677,16 +710,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -697,7 +730,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -708,7 +741,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Added a capacity fix - so that the capacity is filled smoothly
</commit_message>
<xml_diff>
--- a/Exogenous values.xlsx
+++ b/Exogenous values.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31512" yWindow="-660" windowWidth="28032" windowHeight="9420" activeTab="4"/>
+    <workbookView xWindow="-31515" yWindow="-660" windowWidth="28035" windowHeight="9420" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="company" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>total number of companies</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>$/month</t>
+  </si>
+  <si>
+    <t>adjustment time for total utilized capacity</t>
+  </si>
+  <si>
+    <t>Month</t>
   </si>
 </sst>
 </file>
@@ -482,12 +488,12 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -498,7 +504,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -509,7 +515,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -520,7 +526,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -538,18 +544,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -560,7 +566,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -571,7 +577,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -580,6 +586,17 @@
       </c>
       <c r="C3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -591,16 +608,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -611,7 +628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -622,7 +639,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -646,12 +663,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -665,7 +682,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -679,7 +696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -690,7 +707,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -710,16 +727,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -730,7 +747,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -741,7 +758,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Fixed total used capacity and added all of the variables descriptions
Now the model works well, and all of the variables descriptions are added. I had to fix the available capacity and total used capacity as well.
</commit_message>
<xml_diff>
--- a/Exogenous values.xlsx
+++ b/Exogenous values.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31515" yWindow="-660" windowWidth="28035" windowHeight="9420" activeTab="2"/>
+    <workbookView xWindow="-31515" yWindow="-660" windowWidth="28035" windowHeight="9420" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="company" sheetId="1" r:id="rId1"/>
@@ -64,9 +64,6 @@
     <t>Box/Hub</t>
   </si>
   <si>
-    <t>goal</t>
-  </si>
-  <si>
     <t>Dmnl</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>Month</t>
+  </si>
+  <si>
+    <t>average delay time in dropping out</t>
   </si>
 </sst>
 </file>
@@ -482,15 +482,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -501,7 +501,7 @@
         <v>100</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -512,29 +512,40 @@
         <v>0.3</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>0.3</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -563,7 +574,7 @@
         <v>100000</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -574,29 +585,29 @@
         <v>10000</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>0.6</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -606,10 +617,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -639,17 +650,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>0.6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -670,52 +670,52 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>1000</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -738,35 +738,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1">
         <v>100</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>1000000</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the exogenous value file with better numbers and updated the model with a "play around" view
The exogenous file now has better values and I started a mini validation of the values as well.  The model has a new view with some graphs. PROBLEM! I don't know why but I couldn't get the synthesim to work!
</commit_message>
<xml_diff>
--- a/Exogenous values.xlsx
+++ b/Exogenous values.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31515" yWindow="-660" windowWidth="28035" windowHeight="9420" activeTab="3"/>
+    <workbookView xWindow="-31515" yWindow="-660" windowWidth="28035" windowHeight="9420" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="company" sheetId="1" r:id="rId1"/>
-    <sheet name="hubs" sheetId="2" r:id="rId2"/>
-    <sheet name="demand" sheetId="3" r:id="rId3"/>
+    <sheet name="variable assumptions and source" sheetId="6" r:id="rId1"/>
+    <sheet name="company" sheetId="1" r:id="rId2"/>
+    <sheet name="hubs" sheetId="2" r:id="rId3"/>
     <sheet name="cost" sheetId="4" r:id="rId4"/>
     <sheet name="emissions" sheetId="5" r:id="rId5"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>total number of companies</t>
   </si>
@@ -131,13 +131,73 @@
   </si>
   <si>
     <t>average delay time in dropping out</t>
+  </si>
+  <si>
+    <t>Calculating the total demand for stockholm</t>
+  </si>
+  <si>
+    <t>Total population in sweden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total population in stockholm </t>
+  </si>
+  <si>
+    <t>https://worldpopulationreview.com/world-cities/stockholm-population</t>
+  </si>
+  <si>
+    <t>https://worldpopulationreview.com/countries/sweden-population</t>
+  </si>
+  <si>
+    <t>Share of population that lives in Stockholm</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?sa=t&amp;rct=j&amp;q=&amp;esrc=s&amp;source=web&amp;cd=&amp;ved=2ahUKEwiIweHQ2YPzAhXrkIsKHVvbBYgQFnoECAcQAQ&amp;url=https%3A%2F%2Fwww.pts.se%2Fglobalassets%2Fstartpage%2Fdokument%2Ficke-legala-dokument%2Frapporter%2F2020%2Fpost%2Fswedish-postal-market-2020.pdf&amp;usg=AOvVaw2czDNsaHt0Xe07B0P7cw6n</t>
+  </si>
+  <si>
+    <t>Number of parcels in Sweden</t>
+  </si>
+  <si>
+    <t>pg 37</t>
+  </si>
+  <si>
+    <t>Number of letters in Sweden (2019) ??</t>
+  </si>
+  <si>
+    <t>Assumption of parcels in Stockholm per year</t>
+  </si>
+  <si>
+    <t>Assumption of parcels in Stockholm per month</t>
+  </si>
+  <si>
+    <t>Calculating the emission factors</t>
+  </si>
+  <si>
+    <t>Emissions for road freight - light duty vehicles - 2019</t>
+  </si>
+  <si>
+    <t>Total Greenhouse Gases (kt CO2-eqv.)</t>
+  </si>
+  <si>
+    <t>In stockholm</t>
+  </si>
+  <si>
+    <t>per parcel</t>
+  </si>
+  <si>
+    <t>kgCO2-eqv./Parcel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swedish environmental protection agency </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -145,13 +205,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -166,8 +246,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,10 +578,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.625" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10173195</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1656571</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <f>B3/B2</f>
+        <v>0.16283684722449535</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="4">
+        <f>1.8055*10^9</f>
+        <v>1805500000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="4">
+        <f>246*10^6</f>
+        <v>246000000</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="8">
+        <f>B6*B4</f>
+        <v>40057864.417225853</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="6">
+        <f>B7/12</f>
+        <v>3338155.3681021542</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="9">
+        <v>1503.7</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14">
+        <f>B13*B4</f>
+        <v>244.85776717147365</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="4">
+        <f>B14/B8</f>
+        <v>7.3351219512195133E-5</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2">
+        <f>B15*10^6</f>
+        <v>73.351219512195129</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A12:C12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -553,17 +814,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -610,43 +872,26 @@
         <v>29</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B1">
-        <v>10000</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B5" s="3">
+        <f>'variable assumptions and source'!B8</f>
+        <v>3338155.3681021542</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>1000</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B6">
+        <v>300000</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -659,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -728,12 +973,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -752,7 +998,7 @@
         <v>18</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -763,7 +1009,7 @@
         <v>20</v>
       </c>
       <c r="B3">
-        <v>1000000</v>
+        <v>300000000</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>

</xml_diff>